<commit_message>
Atualização automática de SANTANA_DO_LIVRAMENTO.xlsx
</commit_message>
<xml_diff>
--- a/SANTANA_DO_LIVRAMENTO.xlsx
+++ b/SANTANA_DO_LIVRAMENTO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C2B5929-3A47-4F38-8224-184375813F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE628297-EFD4-425F-BA88-1868CAD06A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1282,7 +1282,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{D996050F-3667-4527-A0F9-4EC34FB42FA9}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{3AC9EE71-8755-4564-B447-5A594A6C7966}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1312,10 +1312,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E11B885B-4EBE-473F-93F2-9047E9722552}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{767D8929-E1B9-4BBE-A94E-6A42838FD1CF}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1353,7 +1353,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A50C6526-8E33-48E4-8812-EC057EA13AAF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D37C4FD0-6EC2-4A6B-A58C-28E002E054C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1416,7 +1416,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D624A2E-D9AF-4089-86DE-A838265D4719}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27B1FC9F-69D1-4FA2-9738-C2C40A472815}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1435,7 +1435,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{576CFFFC-39AE-D3AF-5238-75D1E0660871}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1F3524D-EDF9-04CA-F521-100BB5040D6E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1484,7 +1484,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86D77CDA-4751-9766-ED7E-D86F4C644184}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1434678D-F4A7-BEC4-D9BD-39866E8526E6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1503,7 +1503,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D9A2DA2-BEFC-D77A-46ED-FECD5363FABB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B6D1C1A-5559-238A-EB6E-C2B0225D20EB}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1534,7 +1534,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9155BCD9-3DC3-7CD5-E6ED-5E3C16FD1639}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{189724D5-ADC6-1D4B-4B32-C4FDF5EDFB68}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1565,7 +1565,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{948EFD20-159E-A485-BAC8-4D3267A4FE45}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9D0E482-0C62-59A4-8B8C-D6A50F807AAC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1608,7 +1608,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDF5E075-322B-404C-B7F2-875A0AD3013A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AE3F454-3E82-4640-AF2E-4419FEB61C90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1646,7 +1646,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8D7BDB3-396D-496C-9646-D1BC35980B0A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2427A734-CAE8-45CE-92F1-B983BA0D2BAD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1689,7 +1689,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F239703-E7B3-4627-A8AF-066899967918}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DCEFAD5-C078-45A6-9FFB-0A7E32C59288}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2002,7 +2002,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B517C148-2CC1-4BB1-AD78-1D0B440F6060}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{562D08F1-B359-4966-AF12-0822B98BEA33}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>